<commit_message>
Bacterial Abundance 2018 Assignment
</commit_message>
<xml_diff>
--- a/Input_Data/week3/144L_2018_BactAbund.xlsx
+++ b/Input_Data/week3/144L_2018_BactAbund.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasbaetge/GITHUB/eemb144l/Input_Data/week3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sam_c\OneDrive\Documents\GitHub EEMB 144L\144l_students\Input_Data\week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38BB174-D4C5-4F42-AC32-372EA7473B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{C38BB174-D4C5-4F42-AC32-372EA7473B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D34AE745-EB97-4403-8BC5-652221E19DB0}"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="2280" windowWidth="22500" windowHeight="17720" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
+    <workbookView minimized="1" xWindow="2420" yWindow="2420" windowWidth="14400" windowHeight="7360" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="66">
   <si>
     <t>A</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>DNA_SampleID</t>
+  </si>
+  <si>
+    <t>Cells_md_sd</t>
   </si>
 </sst>
 </file>
@@ -589,13 +592,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB9DCA8-3A58-FF4E-A0AD-EB8E080FD40B}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -645,7 +648,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -695,7 +698,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -742,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -789,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -836,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -886,7 +889,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -933,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -980,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1412,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1506,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1603,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1794,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1938,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2035,7 +2038,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -2082,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -2179,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -2273,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -2370,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -2561,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -2611,7 +2614,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -2802,7 +2805,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -2849,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -2943,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -2993,7 +2996,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3040,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -3090,7 +3093,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -3137,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -3231,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -3281,7 +3284,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -3328,7 +3331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3375,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3422,7 +3425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3472,7 +3475,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -3519,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -3569,7 +3572,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -3616,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -3663,7 +3666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -3710,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -3760,7 +3763,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -3807,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -3854,7 +3857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -3951,7 +3954,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -3998,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -4048,7 +4051,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -4095,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>15</v>
       </c>
@@ -4189,7 +4192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>15</v>
       </c>
@@ -4239,7 +4242,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -4286,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -4333,7 +4336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -4380,7 +4383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -4430,7 +4433,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>15</v>
       </c>
@@ -4485,15 +4488,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5332B8C1-55B2-BD48-914B-6263445B7F27}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -4503,8 +4506,11 @@
       <c r="C1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4514,8 +4520,12 @@
       <c r="C2">
         <v>332531.52198164398</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f xml:space="preserve"> STDEVA(C2:C73)</f>
+        <v>362682.87239282375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4526,7 +4536,7 @@
         <v>523943.12466870598</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4537,7 +4547,7 @@
         <v>859019.93419282604</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4548,7 +4558,7 @@
         <v>906998.85629899101</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -4559,7 +4569,7 @@
         <v>933025.23444792104</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4570,7 +4580,7 @@
         <v>861129.08707527199</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -4581,7 +4591,7 @@
         <v>798345.82660480496</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4592,7 +4602,7 @@
         <v>818468.442863937</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -4603,7 +4613,7 @@
         <v>967204.14777526399</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -4614,7 +4624,7 @@
         <v>389243.417879941</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -4625,7 +4635,7 @@
         <v>540180.18661691702</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -4636,7 +4646,7 @@
         <v>703840.6175089</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -4647,7 +4657,7 @@
         <v>974216.42015463102</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -4658,7 +4668,7 @@
         <v>1106511.5789880999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -4669,7 +4679,7 @@
         <v>1017122.84270029</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -4680,7 +4690,7 @@
         <v>1020031.54746963</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -4691,7 +4701,7 @@
         <v>927016.18583212199</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -4702,7 +4712,7 @@
         <v>826944.80386336998</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -4713,7 +4723,7 @@
         <v>336545.30778626399</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -4724,7 +4734,7 @@
         <v>996356.76683978795</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -4735,7 +4745,7 @@
         <v>1230196.2472266301</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -4746,7 +4756,7 @@
         <v>1302477.9536003701</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -4757,7 +4767,7 @@
         <v>1371723.38387575</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -4768,7 +4778,7 @@
         <v>1374719.18912593</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -4779,7 +4789,7 @@
         <v>1082805.7139993799</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -4790,7 +4800,7 @@
         <v>700633.12558165798</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -4801,7 +4811,7 @@
         <v>269659.90008467803</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -4812,7 +4822,7 @@
         <v>378432.32852996897</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -4823,7 +4833,7 @@
         <v>1143848.3877767001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -4834,7 +4844,7 @@
         <v>1284329.8248072199</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -4845,7 +4855,7 @@
         <v>1491056.04413508</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -4856,7 +4866,7 @@
         <v>1282878.1580936001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -4867,7 +4877,7 @@
         <v>1382528.67009801</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -4878,7 +4888,7 @@
         <v>1243556.81129429</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -4889,7 +4899,7 @@
         <v>635058.66244288802</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -4900,7 +4910,7 @@
         <v>303070.34540015197</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -4911,7 +4921,7 @@
         <v>340956.94619767403</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -4922,7 +4932,7 @@
         <v>635639.45786774298</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -4933,7 +4943,7 @@
         <v>832832.30079724698</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -4944,7 +4954,7 @@
         <v>908466.52265596495</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -4955,7 +4965,7 @@
         <v>860914.43198922602</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -4966,7 +4976,7 @@
         <v>960415.60478444002</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -4977,7 +4987,7 @@
         <v>1078301.7794102</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -4988,7 +4998,7 @@
         <v>1037393.33704528</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -4999,7 +5009,7 @@
         <v>839206.07339605805</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -5010,7 +5020,7 @@
         <v>337723.07982937701</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -5021,7 +5031,7 @@
         <v>629380.28959407099</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -5032,7 +5042,7 @@
         <v>902830.40902295697</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -5043,7 +5053,7 @@
         <v>901296.45391014102</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -5054,7 +5064,7 @@
         <v>839401.52858474804</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -5065,7 +5075,7 @@
         <v>920903.92715527106</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -5076,7 +5086,7 @@
         <v>933577.68101578299</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -5087,7 +5097,7 @@
         <v>980723.44291230396</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -5098,7 +5108,7 @@
         <v>843245.801244242</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -5109,7 +5119,7 @@
         <v>328736.07934774499</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -5120,7 +5130,7 @@
         <v>606397.36670402798</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -5131,7 +5141,7 @@
         <v>1373083.2977872901</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -5142,7 +5152,7 @@
         <v>1221161.3344965</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -5153,7 +5163,7 @@
         <v>1359810.73724745</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -5164,7 +5174,7 @@
         <v>1365703.6299326799</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -5175,7 +5185,7 @@
         <v>1286004.58111447</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -5186,7 +5196,7 @@
         <v>950166.57041443698</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -5197,7 +5207,7 @@
         <v>311668.24715130503</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -5208,7 +5218,7 @@
         <v>352672.90218353103</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -5219,7 +5229,7 @@
         <v>614087.59233860904</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -5230,7 +5240,7 @@
         <v>1366410.8793915799</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -5241,7 +5251,7 @@
         <v>1312103.0477472299</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -5252,7 +5262,7 @@
         <v>1619535.40675905</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -5263,7 +5273,7 @@
         <v>1559568.28414247</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -5274,7 +5284,7 @@
         <v>1506645.1241826899</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -5285,7 +5295,7 @@
         <v>856541.22968476801</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>7</v>
       </c>

</xml_diff>